<commit_message>
Fifth commit - Some test cases are added...
</commit_message>
<xml_diff>
--- a/TestData/createWaveWithHost.xlsx
+++ b/TestData/createWaveWithHost.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pranav Pawar\PycharmProjects\RMM_DataDriven\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CAE496A-64FE-44CE-B895-B2ECFF399D20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F437C019-62E6-4DB2-B77F-11497B202B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4380" yWindow="2556" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t>Wave Name</t>
   </si>
@@ -83,112 +83,91 @@
     <t xml:space="preserve">Target - SSH Port </t>
   </si>
   <si>
-    <t>winStage1</t>
-  </si>
-  <si>
-    <t>winStage2</t>
-  </si>
-  <si>
-    <t>winStage12</t>
-  </si>
-  <si>
-    <t>linStage1</t>
-  </si>
-  <si>
-    <t>linStage2</t>
-  </si>
-  <si>
-    <t>linStage12</t>
-  </si>
-  <si>
-    <t>Autoprovision</t>
-  </si>
-  <si>
-    <t>11.0.0.1</t>
-  </si>
-  <si>
-    <t>11.0.0.2</t>
-  </si>
-  <si>
-    <t>11.0.0.12</t>
-  </si>
-  <si>
-    <t>12.0.0.1</t>
-  </si>
-  <si>
-    <t>12.0.0.2</t>
-  </si>
-  <si>
-    <t>winStage1-src</t>
-  </si>
-  <si>
-    <t>winStage2-src</t>
-  </si>
-  <si>
-    <t>winStage12-src</t>
-  </si>
-  <si>
-    <t>linStage1-src</t>
-  </si>
-  <si>
-    <t>linStage2-src</t>
-  </si>
-  <si>
-    <t>linStage12-src</t>
-  </si>
-  <si>
-    <t>Windows</t>
-  </si>
-  <si>
     <t>Linux</t>
   </si>
   <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>Stage 1</t>
-  </si>
-  <si>
-    <t>Stage 2</t>
-  </si>
-  <si>
-    <t>Stage 1 &amp; 2</t>
-  </si>
-  <si>
-    <t>winStage1-tgt</t>
-  </si>
-  <si>
-    <t>winStage2-tgt</t>
-  </si>
-  <si>
-    <t>winStage12-tgt</t>
-  </si>
-  <si>
-    <t>linStage1-tgt</t>
-  </si>
-  <si>
-    <t>linStage2-tgt</t>
-  </si>
-  <si>
-    <t>linStage12-tgt</t>
-  </si>
-  <si>
-    <t>winStage1-img</t>
-  </si>
-  <si>
-    <t>winStage2-img</t>
-  </si>
-  <si>
-    <t>winStage12-img</t>
-  </si>
-  <si>
-    <t>linStage1-img</t>
-  </si>
-  <si>
-    <t>linStage2-img</t>
-  </si>
-  <si>
-    <t>linStage12-img</t>
+    <t>Common Data</t>
+  </si>
+  <si>
+    <t>Source Data</t>
+  </si>
+  <si>
+    <t>Target Data</t>
+  </si>
+  <si>
+    <t>TNG</t>
+  </si>
+  <si>
+    <t>Verbose</t>
+  </si>
+  <si>
+    <t>Allow Direct FSCopy</t>
+  </si>
+  <si>
+    <t>Allow FS Deletion</t>
+  </si>
+  <si>
+    <t>No Transfer</t>
+  </si>
+  <si>
+    <t>Transfer Compress</t>
+  </si>
+  <si>
+    <t>No Transfer Compress</t>
+  </si>
+  <si>
+    <t>Ignore Missing</t>
+  </si>
+  <si>
+    <t>No In Place</t>
+  </si>
+  <si>
+    <t>No Reboot</t>
+  </si>
+  <si>
+    <t>Include SAN</t>
+  </si>
+  <si>
+    <t>Exclude SAN</t>
+  </si>
+  <si>
+    <t>Override RMM Storage Check</t>
+  </si>
+  <si>
+    <t>Delete All Target FS</t>
+  </si>
+  <si>
+    <t>Keep Target Layout</t>
+  </si>
+  <si>
+    <t>Cloud Init</t>
+  </si>
+  <si>
+    <t>Sync Options</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Existing System</t>
+  </si>
+  <si>
+    <t>172.29.31.111</t>
+  </si>
+  <si>
+    <t>psp-my-src</t>
+  </si>
+  <si>
+    <t>root</t>
+  </si>
+  <si>
+    <t>Direct Sync</t>
+  </si>
+  <si>
+    <t>psp-my-tgt</t>
+  </si>
+  <si>
+    <t>172.29.30.130</t>
   </si>
 </sst>
 </file>
@@ -238,9 +217,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -521,307 +506,240 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:AE3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20.21875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.77734375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="27.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="27.21875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.21875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="3"/>
+      <c r="AC1" s="3"/>
+      <c r="AD1" s="3"/>
+      <c r="AE1" s="3"/>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="P2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="b">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2">
-        <v>22</v>
-      </c>
-      <c r="H2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I2" t="s">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>36</v>
-      </c>
-      <c r="J2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K2" t="s">
-        <v>45</v>
-      </c>
-      <c r="O2">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>16</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="G3">
         <v>22</v>
       </c>
       <c r="H3" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="I3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="J3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" t="s">
+        <v>43</v>
+      </c>
+      <c r="M3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N3" t="s">
         <v>40</v>
-      </c>
-      <c r="K3" t="s">
-        <v>46</v>
       </c>
       <c r="O3">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" t="b">
+      <c r="Q3" t="b">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4">
-        <v>22</v>
-      </c>
-      <c r="H4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I4" t="s">
-        <v>38</v>
-      </c>
-      <c r="J4" t="s">
-        <v>41</v>
-      </c>
-      <c r="K4" t="s">
-        <v>47</v>
-      </c>
-      <c r="O4">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="b">
+      <c r="R3" t="b">
         <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5">
-        <v>22</v>
-      </c>
-      <c r="H5" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" t="s">
-        <v>36</v>
-      </c>
-      <c r="J5" t="s">
-        <v>42</v>
-      </c>
-      <c r="K5" t="s">
-        <v>48</v>
-      </c>
-      <c r="O5">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6">
-        <v>22</v>
-      </c>
-      <c r="H6" t="s">
-        <v>35</v>
-      </c>
-      <c r="I6" t="s">
-        <v>37</v>
-      </c>
-      <c r="J6" t="s">
-        <v>43</v>
-      </c>
-      <c r="K6" t="s">
-        <v>49</v>
-      </c>
-      <c r="O6">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" t="b">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7">
-        <v>22</v>
-      </c>
-      <c r="H7" t="s">
-        <v>35</v>
-      </c>
-      <c r="I7" t="s">
-        <v>38</v>
-      </c>
-      <c r="J7" t="s">
-        <v>44</v>
-      </c>
-      <c r="K7" t="s">
-        <v>50</v>
-      </c>
-      <c r="O7">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="J1:O1"/>
+    <mergeCell ref="P1:AE1"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>